<commit_message>
added desription to parameter list
</commit_message>
<xml_diff>
--- a/parameter_list/all_covidsim_params.xlsx
+++ b/parameter_list/all_covidsim_params.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="all_params" sheetId="1" state="visible" r:id="rId2"/>
@@ -3839,7 +3839,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>7529040</xdr:colOff>
+      <xdr:colOff>7528680</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>111240</xdr:rowOff>
     </xdr:to>
@@ -3851,7 +3851,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7844400" y="660960"/>
-          <a:ext cx="5207040" cy="2863800"/>
+          <a:ext cx="5206680" cy="2863800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4028,16 +4028,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>812880</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>66240</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>720</xdr:rowOff>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>690480</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>763560</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4046,8 +4046,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9051840" y="163080"/>
-          <a:ext cx="5611680" cy="1684440"/>
+          <a:off x="10377720" y="190080"/>
+          <a:ext cx="5619960" cy="1684440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4153,11 +4153,11 @@
   </sheetPr>
   <dimension ref="A1:D941"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A497" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A530" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D535" activeCellId="0" sqref="D535"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="78.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="130.6"/>
@@ -17252,13 +17252,13 @@
   </sheetPr>
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J21" activeCellId="0" sqref="J21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="64.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.54"/>
   </cols>
   <sheetData>
@@ -17716,7 +17716,7 @@
         <v>1.5</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>1180</v>
+        <v>174</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>1182</v>

</xml_diff>